<commit_message>
cleaned up graphs and links
</commit_message>
<xml_diff>
--- a/2014-01-16 Football Hometowns/tables.xlsx
+++ b/2014-01-16 Football Hometowns/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="24460" windowHeight="16920" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="24460" windowHeight="16920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="concentration" sheetId="1" r:id="rId1"/>
@@ -20,38 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
-  <si>
-    <t>Northern Arizona Lumberjacks</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Houston Baptist Huskies</t>
   </si>
   <si>
-    <t>Hawaii Warriors</t>
-  </si>
-  <si>
-    <t>Central Connecticut State Blue Devils</t>
-  </si>
-  <si>
-    <t>USC Trojans</t>
-  </si>
-  <si>
-    <t>Houston Cougars</t>
-  </si>
-  <si>
-    <t>San Diego State Aztecs</t>
-  </si>
-  <si>
     <t>Pittsburgh Panthers</t>
   </si>
   <si>
-    <t>Washington Huskies</t>
-  </si>
-  <si>
-    <t>San Diego Toreros</t>
-  </si>
-  <si>
     <t>Louisville Cardinals</t>
   </si>
   <si>
@@ -121,9 +97,6 @@
     <t>Iowa Hawkeyes</t>
   </si>
   <si>
-    <t>Lehigh Mountain Hawks</t>
-  </si>
-  <si>
     <t>Cornell Big Red</t>
   </si>
   <si>
@@ -136,12 +109,6 @@
     <t>Princeton Tigers</t>
   </si>
   <si>
-    <t>Elon Phoenix</t>
-  </si>
-  <si>
-    <t>Wofford Terriers</t>
-  </si>
-  <si>
     <t>Harvard Crimson</t>
   </si>
   <si>
@@ -157,13 +124,55 @@
     <t>Top 15 Heaviest Teams</t>
   </si>
   <si>
-    <t>Top 25 team</t>
-  </si>
-  <si>
-    <t>Top 10 Least Geographically Diverse</t>
-  </si>
-  <si>
-    <t>Top 10 Most Geographically Diverse</t>
+    <t>Football Teams Ranked by Geographic Diversity</t>
+  </si>
+  <si>
+    <t>Dartmouth Big Green</t>
+  </si>
+  <si>
+    <t>Georgetown Hoyas</t>
+  </si>
+  <si>
+    <t>Columbia Lions</t>
+  </si>
+  <si>
+    <t>Yale Bulldogs</t>
+  </si>
+  <si>
+    <t>Florida State Seminoles</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>North Texas Mean Green</t>
+  </si>
+  <si>
+    <t>Lamar Cardinals</t>
+  </si>
+  <si>
+    <t>Texas Longhorns</t>
+  </si>
+  <si>
+    <t>Sacramento State Hornets</t>
+  </si>
+  <si>
+    <t>Cal Poly Mustangs</t>
+  </si>
+  <si>
+    <t>Sam Houston State Bearkats</t>
+  </si>
+  <si>
+    <t>Incarnate Word Cardinals</t>
+  </si>
+  <si>
+    <t>Stephen F. Austin Lumberjacks</t>
+  </si>
+  <si>
+    <t>UC Davis Aggies</t>
+  </si>
+  <si>
+    <t>Top 25 teams shown in green</t>
   </si>
 </sst>
 </file>
@@ -256,7 +265,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -290,13 +299,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -304,12 +322,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -326,8 +338,29 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -344,6 +377,11 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -360,6 +398,11 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -689,215 +732,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:G13"/>
+  <dimension ref="C1:E30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" customWidth="1"/>
-    <col min="5" max="6" width="4.1640625" customWidth="1"/>
-    <col min="7" max="7" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" ht="18" customHeight="1">
-      <c r="C1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="13"/>
-    </row>
-    <row r="2" spans="3:7" ht="31" customHeight="1">
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-    </row>
-    <row r="4" spans="3:7" ht="16">
-      <c r="C4" s="16" t="str">
+    <row r="1" spans="3:5" ht="18" customHeight="1">
+      <c r="C1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="3:5" ht="31" customHeight="1">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="4" spans="3:5" ht="16">
+      <c r="C4" s="19" t="str">
         <f>"1."</f>
         <v>1.</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>0</v>
+      <c r="D4" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="16" t="str">
-        <f>"1."</f>
-        <v>1.</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" ht="16">
-      <c r="C5" s="17" t="str">
+    </row>
+    <row r="5" spans="3:5" ht="16">
+      <c r="C5" s="20" t="str">
         <f>"2."</f>
         <v>2.</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>1</v>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="17" t="str">
-        <f>"2."</f>
-        <v>2.</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="16">
-      <c r="C6" s="17" t="str">
+    </row>
+    <row r="6" spans="3:5" ht="16">
+      <c r="C6" s="20" t="str">
         <f>"3."</f>
         <v>3.</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>2</v>
+      <c r="D6" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="17" t="str">
-        <f>"3."</f>
-        <v>3.</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="16">
-      <c r="C7" s="17" t="str">
+    </row>
+    <row r="7" spans="3:5" ht="16">
+      <c r="C7" s="20" t="str">
         <f>"4."</f>
         <v>4.</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>3</v>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="17" t="str">
-        <f>"4."</f>
-        <v>4.</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="16">
-      <c r="C8" s="17" t="str">
+    </row>
+    <row r="8" spans="3:5" ht="16">
+      <c r="C8" s="20" t="str">
         <f>"5."</f>
         <v>5.</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>4</v>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="17" t="str">
-        <f>"5."</f>
-        <v>5.</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="16">
-      <c r="C9" s="17" t="str">
+    </row>
+    <row r="9" spans="3:5" ht="16">
+      <c r="C9" s="20" t="str">
         <f>"6."</f>
         <v>6.</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>5</v>
+      <c r="D9" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="17" t="str">
-        <f>"6."</f>
-        <v>6.</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="16">
-      <c r="C10" s="17" t="str">
+    </row>
+    <row r="10" spans="3:5" ht="16">
+      <c r="C10" s="20" t="str">
         <f>"7."</f>
         <v>7.</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>6</v>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="17" t="str">
-        <f>"7."</f>
-        <v>7.</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="16">
-      <c r="C11" s="17" t="str">
+    </row>
+    <row r="11" spans="3:5" ht="16">
+      <c r="C11" s="20" t="str">
         <f>"8."</f>
         <v>8.</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="17" t="str">
-        <f>"8."</f>
-        <v>8.</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="16">
-      <c r="C12" s="17" t="str">
+    </row>
+    <row r="12" spans="3:5" ht="16">
+      <c r="C12" s="20" t="str">
         <f>"9."</f>
         <v>9.</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>8</v>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="17" t="str">
-        <f>"9."</f>
-        <v>9.</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="16">
-      <c r="C13" s="18" t="str">
+    </row>
+    <row r="13" spans="3:5" ht="16">
+      <c r="C13" s="20" t="str">
         <f>"10."</f>
         <v>10.</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>9</v>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="18" t="str">
-        <f>"10."</f>
-        <v>10.</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>33</v>
+    </row>
+    <row r="14" spans="3:5" ht="19" customHeight="1">
+      <c r="C14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="22"/>
+    </row>
+    <row r="15" spans="3:5" ht="16">
+      <c r="C15" s="21" t="str">
+        <f>"21."</f>
+        <v>21.</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" ht="16">
+      <c r="C16" s="21" t="str">
+        <f>"54."</f>
+        <v>54.</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="16">
+      <c r="C17" s="21" t="str">
+        <f>"96."</f>
+        <v>96.</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="16">
+      <c r="C18" s="21" t="str">
+        <f>"136."</f>
+        <v>136.</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="16">
+      <c r="C19" s="21" t="str">
+        <f>"219."</f>
+        <v>219.</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="19" customHeight="1">
+      <c r="C20" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" spans="3:4" ht="16">
+      <c r="C21" s="21" t="str">
+        <f>"242."</f>
+        <v>242.</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" ht="16">
+      <c r="C22" s="21" t="str">
+        <f>"243."</f>
+        <v>243.</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" ht="16">
+      <c r="C23" s="21" t="str">
+        <f>"244."</f>
+        <v>244.</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" ht="16">
+      <c r="C24" s="21" t="str">
+        <f>"245."</f>
+        <v>245.</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" ht="16">
+      <c r="C25" s="21" t="str">
+        <f>"246."</f>
+        <v>246.</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" ht="16">
+      <c r="C26" s="21" t="str">
+        <f>"247."</f>
+        <v>247.</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" ht="16">
+      <c r="C27" s="21" t="str">
+        <f>"248."</f>
+        <v>248.</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" ht="16">
+      <c r="C28" s="21" t="str">
+        <f>"249."</f>
+        <v>249.</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" ht="16">
+      <c r="C29" s="21" t="str">
+        <f>"250."</f>
+        <v>250.</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" ht="16">
+      <c r="C30" s="23" t="str">
+        <f>"251."</f>
+        <v>251.</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="G2:H11">
-    <sortCondition ref="H2"/>
+  <sortState ref="F2:H11">
+    <sortCondition ref="F2"/>
   </sortState>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C1:D2"/>
-    <mergeCell ref="F1:G2"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -914,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F29"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -929,15 +1044,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="18">
-      <c r="B3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="12"/>
+      <c r="B3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="17"/>
     </row>
     <row r="4" spans="2:6" ht="16">
       <c r="C4" s="2"/>
@@ -946,263 +1061,263 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="2:6" ht="16">
-      <c r="B5" s="16" t="str">
+      <c r="B5" s="13" t="str">
         <f>"1."</f>
         <v>1.</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>29</v>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="16" t="str">
+      <c r="E5" s="13" t="str">
         <f>"1."</f>
         <v>1.</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>27</v>
+      <c r="F5" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="16">
-      <c r="B6" s="17" t="str">
+      <c r="B6" s="14" t="str">
         <f>"2."</f>
         <v>2.</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>25</v>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="17" t="str">
+      <c r="E6" s="14" t="str">
         <f>"2."</f>
         <v>2.</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>29</v>
+      <c r="F6" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="16">
-      <c r="B7" s="17" t="str">
+      <c r="B7" s="14" t="str">
         <f>"3."</f>
         <v>3.</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>26</v>
+      <c r="C7" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="17" t="str">
+      <c r="E7" s="14" t="str">
         <f>"3."</f>
         <v>3.</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>16</v>
+      <c r="F7" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="16">
-      <c r="B8" s="17" t="str">
+      <c r="B8" s="14" t="str">
         <f>"4."</f>
         <v>4.</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>22</v>
+      <c r="C8" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="17" t="str">
+      <c r="E8" s="14" t="str">
         <f>"4."</f>
         <v>4.</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>30</v>
+      <c r="F8" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="16">
-      <c r="B9" s="17" t="str">
+      <c r="B9" s="14" t="str">
         <f>"5."</f>
         <v>5.</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
+      <c r="C9" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="17" t="str">
+      <c r="E9" s="14" t="str">
         <f>"5."</f>
         <v>5.</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>14</v>
+      <c r="F9" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="16">
-      <c r="B10" s="17" t="str">
+      <c r="B10" s="14" t="str">
         <f>"6."</f>
         <v>6.</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>28</v>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="17" t="str">
+      <c r="E10" s="14" t="str">
         <f>"6."</f>
         <v>6.</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>35</v>
+      <c r="F10" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="16">
-      <c r="B11" s="17" t="str">
+      <c r="B11" s="14" t="str">
         <f>"7."</f>
         <v>7.</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>13</v>
+      <c r="C11" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="17" t="str">
+      <c r="E11" s="14" t="str">
         <f>"7."</f>
         <v>7.</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>10</v>
+      <c r="F11" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="16">
-      <c r="B12" s="17" t="str">
+      <c r="B12" s="14" t="str">
         <f>"8."</f>
         <v>8.</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>15</v>
+      <c r="C12" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="17" t="str">
+      <c r="E12" s="14" t="str">
         <f>"8."</f>
         <v>8.</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>31</v>
+      <c r="F12" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="16">
-      <c r="B13" s="17" t="str">
+      <c r="B13" s="14" t="str">
         <f>"9."</f>
         <v>9.</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>14</v>
+      <c r="C13" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="17" t="str">
+      <c r="E13" s="14" t="str">
         <f>"9."</f>
         <v>9.</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>18</v>
+      <c r="F13" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="16">
-      <c r="B14" s="17" t="str">
+      <c r="B14" s="14" t="str">
         <f>"10."</f>
         <v>10.</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>32</v>
+      <c r="C14" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="17" t="str">
+      <c r="E14" s="14" t="str">
         <f>"10."</f>
         <v>10.</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>20</v>
+      <c r="F14" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="16">
-      <c r="B15" s="17" t="str">
+      <c r="B15" s="14" t="str">
         <f>"11."</f>
         <v>11.</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>17</v>
+      <c r="C15" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="17" t="str">
+      <c r="E15" s="14" t="str">
         <f>"11."</f>
         <v>11.</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>19</v>
+      <c r="F15" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="16">
-      <c r="B16" s="17" t="str">
+      <c r="B16" s="14" t="str">
         <f>"12."</f>
         <v>12.</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>23</v>
+      <c r="C16" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="D16" s="3"/>
-      <c r="E16" s="17" t="str">
+      <c r="E16" s="14" t="str">
         <f>"12."</f>
         <v>12.</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>7</v>
+      <c r="F16" s="5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="16">
-      <c r="B17" s="17" t="str">
+      <c r="B17" s="14" t="str">
         <f>"13."</f>
         <v>13.</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>27</v>
+      <c r="C17" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="17" t="str">
+      <c r="E17" s="14" t="str">
         <f>"13."</f>
         <v>13.</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>21</v>
+      <c r="F17" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="16">
-      <c r="B18" s="17" t="str">
+      <c r="B18" s="14" t="str">
         <f>"14."</f>
         <v>14.</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>34</v>
+      <c r="C18" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="17" t="str">
+      <c r="E18" s="14" t="str">
         <f>"14."</f>
         <v>14.</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>11</v>
+      <c r="F18" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="16">
-      <c r="B19" s="18" t="str">
+      <c r="B19" s="15" t="str">
         <f>"15."</f>
         <v>15.</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>30</v>
+      <c r="C19" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="18" t="str">
+      <c r="E19" s="15" t="str">
         <f>"15."</f>
         <v>15.</v>
       </c>
-      <c r="F19" s="11" t="s">
-        <v>24</v>
+      <c r="F19" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="16">
-      <c r="C21" s="4" t="s">
-        <v>45</v>
+      <c r="C21" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:6">

</xml_diff>